<commit_message>
Update Python script to point to most recent risk table version. Generate a new Master_NCI_Risk_Table.xlsx file.
</commit_message>
<xml_diff>
--- a/risk-tables/output/Master_NCI_Risk_Table.xlsx
+++ b/risk-tables/output/Master_NCI_Risk_Table.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="57">
   <si>
     <t>PAST HISTORY (most recent)</t>
   </si>
@@ -131,7 +131,7 @@
     <t>CIN3+ 1 year risk  (%)</t>
   </si>
   <si>
-    <t>HPV-positive NILM</t>
+    <t>HPV-positive NILM x2</t>
   </si>
   <si>
     <t>HPV-positive ASC-US</t>
@@ -170,7 +170,7 @@
     <t>Low Grade</t>
   </si>
   <si>
-    <t xml:space="preserve"> HPV-negative/ASCUS/LSIL</t>
+    <t xml:space="preserve"> HPV-negative/ASC-US/LSIL</t>
   </si>
   <si>
     <t>HPV-negative x2</t>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>Biopsy Result Before Treatment</t>
+  </si>
+  <si>
+    <t>CIN 2 or 3</t>
   </si>
   <si>
     <t>HPV-negative x3</t>
@@ -4198,7 +4201,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -4218,7 +4221,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -4238,7 +4241,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -4258,7 +4261,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -4278,7 +4281,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -4298,7 +4301,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -4318,7 +4321,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -4338,7 +4341,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
         <v>51</v>
@@ -4355,7 +4358,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
         <v>52</v>
@@ -4372,10 +4375,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D11">
         <v>0.15</v>
@@ -4389,10 +4392,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D12">
         <v>0</v>

</xml_diff>